<commit_message>
updated spreadsheeet to have latest SPARTA information
</commit_message>
<xml_diff>
--- a/doc/sphinx/00_intro/SSNI-baseline-draft.xlsx
+++ b/doc/sphinx/00_intro/SSNI-baseline-draft.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gshipman/Documents/sid/ats-5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amagela/Work/git/lanl-benchmarks-ultima01/doc/sphinx/00_intro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CD0C2D-F9A3-7B4F-BA7B-D5C7A832BA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813C3C57-410E-7649-8D79-D8418B78142A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29220" yWindow="33500" windowWidth="23540" windowHeight="19420" xr2:uid="{CE21BE01-DC02-494E-9954-4C73F5D14895}"/>
+    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{CE21BE01-DC02-494E-9954-4C73F5D14895}"/>
   </bookViews>
   <sheets>
     <sheet name="xROADS-Intel-SPR-HBM" sheetId="2" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t xml:space="preserve">40% Memory xROADS </t>
   </si>
   <si>
-    <t>ppc=35</t>
-  </si>
-  <si>
     <t xml:space="preserve">Example 1 - assumes 18k nodes each with 4x improvement across all benchmarks </t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t xml:space="preserve">SSNI baseline draft </t>
+  </si>
+  <si>
+    <t>ppc=55</t>
   </si>
 </sst>
 </file>
@@ -215,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -223,13 +223,12 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,7 +546,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,18 +555,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>36</v>
+      <c r="A1" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>4.0919999999999996</v>
@@ -575,11 +574,11 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="10"/>
     </row>
@@ -607,7 +606,7 @@
         <v>6</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>18</v>
@@ -627,22 +626,22 @@
         <v>18000</v>
       </c>
       <c r="E7" s="5">
-        <f>C7*$B$4</f>
+        <f t="shared" ref="E7:E16" si="0">C7*$B$4</f>
         <v>3924227.9999999995</v>
       </c>
       <c r="F7" s="3">
         <v>0.1</v>
       </c>
       <c r="G7" s="5">
-        <f>E7/C7</f>
+        <f t="shared" ref="G7:G16" si="1">E7/C7</f>
         <v>4.0919999999999996</v>
       </c>
       <c r="H7" s="3">
-        <f>D7/B7</f>
+        <f t="shared" ref="H7:H16" si="2">D7/B7</f>
         <v>2.9315960912052117</v>
       </c>
       <c r="I7" s="6">
-        <f>F7*LN(G7)</f>
+        <f t="shared" ref="I7:I16" si="3">F7*LN(G7)</f>
         <v>0.14090338480893802</v>
       </c>
       <c r="J7" t="s">
@@ -663,22 +662,22 @@
         <v>18000</v>
       </c>
       <c r="E8" s="5">
-        <f>C8*$B$4</f>
+        <f t="shared" si="0"/>
         <v>1677310799.9999998</v>
       </c>
       <c r="F8" s="3">
         <v>0.05</v>
       </c>
       <c r="G8" s="5">
-        <f>E8/C8</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H8" s="3">
-        <f>D8/B8</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I8" s="6">
-        <f>F8*LN(G8)</f>
+        <f t="shared" si="3"/>
         <v>7.045169240446901E-2</v>
       </c>
       <c r="J8" t="s">
@@ -699,22 +698,22 @@
         <v>18000</v>
       </c>
       <c r="E9" s="5">
-        <f>C9*$B$4</f>
+        <f t="shared" si="0"/>
         <v>425608919.99999994</v>
       </c>
       <c r="F9" s="3">
         <v>0.05</v>
       </c>
       <c r="G9" s="5">
-        <f>E9/C9</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H9" s="3">
-        <f>D9/B9</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I9" s="6">
-        <f>F9*LN(G9)</f>
+        <f t="shared" si="3"/>
         <v>7.045169240446901E-2</v>
       </c>
       <c r="J9" t="s">
@@ -735,22 +734,22 @@
         <v>18000</v>
       </c>
       <c r="E10" s="5">
-        <f>C10*$B$4</f>
+        <f t="shared" si="0"/>
         <v>37605.684599999993</v>
       </c>
       <c r="F10" s="3">
         <v>0.15</v>
       </c>
       <c r="G10" s="5">
-        <f>E10/C10</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H10" s="3">
-        <f>D10/B10</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I10" s="6">
-        <f>F10*LN(G10)</f>
+        <f t="shared" si="3"/>
         <v>0.21135507721340699</v>
       </c>
       <c r="J10" t="s">
@@ -764,7 +763,7 @@
       <c r="B11" s="3">
         <v>6140</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11">
         <f>1/2.63468153</f>
         <v>0.37955251464491041</v>
       </c>
@@ -772,22 +771,22 @@
         <v>18000</v>
       </c>
       <c r="E11" s="5">
-        <f>C11*$B$4</f>
+        <f t="shared" si="0"/>
         <v>1.5531288899269733</v>
       </c>
       <c r="F11" s="3">
         <v>0.05</v>
       </c>
       <c r="G11" s="5">
-        <f>E11/C11</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H11" s="3">
-        <f>D11/B11</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I11" s="6">
-        <f>F11*LN(G11)</f>
+        <f t="shared" si="3"/>
         <v>7.045169240446901E-2</v>
       </c>
       <c r="J11" t="s">
@@ -808,22 +807,22 @@
         <v>18000</v>
       </c>
       <c r="E12" s="5">
-        <f>C12*$B$4</f>
+        <f t="shared" si="0"/>
         <v>4939.0439999999999</v>
       </c>
       <c r="F12" s="3">
         <v>0.05</v>
       </c>
       <c r="G12" s="5">
-        <f>E12/C12</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H12" s="3">
-        <f>D12/B12</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I12" s="6">
-        <f>F12*LN(G12)</f>
+        <f t="shared" si="3"/>
         <v>7.045169240446901E-2</v>
       </c>
       <c r="J12" t="s">
@@ -837,29 +836,29 @@
       <c r="B13" s="3">
         <v>6140</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>20000000</v>
       </c>
       <c r="D13" s="3">
         <v>18000</v>
       </c>
       <c r="E13" s="5">
-        <f>C13*$B$4</f>
+        <f t="shared" si="0"/>
         <v>81840000</v>
       </c>
       <c r="F13" s="3">
         <v>0.3</v>
       </c>
       <c r="G13" s="5">
-        <f>E13/C13</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H13" s="3">
-        <f>D13/B13</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I13" s="6">
-        <f>F13*LN(G13)</f>
+        <f t="shared" si="3"/>
         <v>0.42271015442681398</v>
       </c>
       <c r="J13" t="s">
@@ -873,33 +872,33 @@
       <c r="B14" s="3">
         <v>6140</v>
       </c>
-      <c r="C14" s="7">
-        <v>2394.9</v>
+      <c r="C14">
+        <v>2522.1403676464702</v>
       </c>
       <c r="D14" s="3">
         <v>18000</v>
       </c>
       <c r="E14" s="5">
-        <f>C14*$B$4</f>
-        <v>9799.9308000000001</v>
+        <f t="shared" si="0"/>
+        <v>10320.598384409355</v>
       </c>
       <c r="F14" s="3">
         <v>0.1</v>
       </c>
       <c r="G14" s="5">
-        <f>E14/C14</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H14" s="3">
-        <f>D14/B14</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I14" s="6">
-        <f>F14*LN(G14)</f>
+        <f t="shared" si="3"/>
         <v>0.14090338480893802</v>
       </c>
       <c r="J14" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -909,33 +908,33 @@
       <c r="B15" s="3">
         <v>6140</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>621330000</v>
       </c>
       <c r="D15" s="3">
         <v>18000</v>
       </c>
       <c r="E15" s="5">
-        <f>C15*$B$4</f>
+        <f t="shared" si="0"/>
         <v>2542482360</v>
       </c>
       <c r="F15" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G15" s="5">
-        <f>E15/C15</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H15" s="3">
-        <f>D15/B15</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I15" s="6">
-        <f>F15*LN(G15)</f>
+        <f t="shared" si="3"/>
         <v>0.10567753860670349</v>
       </c>
       <c r="J15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -945,33 +944,33 @@
       <c r="B16" s="3">
         <v>6140</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>391002000</v>
       </c>
       <c r="D16" s="3">
         <v>18000</v>
       </c>
       <c r="E16" s="5">
-        <f>C16*$B$4</f>
+        <f t="shared" si="0"/>
         <v>1599980183.9999998</v>
       </c>
       <c r="F16" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G16" s="5">
-        <f>E16/C16</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H16" s="3">
-        <f>D16/B16</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I16" s="6">
-        <f>F16*LN(G16)</f>
+        <f t="shared" si="3"/>
         <v>0.10567753860670349</v>
       </c>
       <c r="J16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -991,12 +990,12 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="3">
         <v>17.989999999999998</v>
@@ -1005,11 +1004,11 @@
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="10"/>
     </row>
@@ -1037,7 +1036,7 @@
         <v>6</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>18</v>
@@ -1057,22 +1056,22 @@
         <v>4096</v>
       </c>
       <c r="E23" s="5">
-        <f>C23*$B$20</f>
+        <f t="shared" ref="E23:E32" si="4">C23*$B$20</f>
         <v>17252410</v>
       </c>
       <c r="F23" s="3">
         <v>0.1</v>
       </c>
       <c r="G23" s="5">
-        <f>E23/C23</f>
+        <f t="shared" ref="G23:G32" si="5">E23/C23</f>
         <v>17.989999999999998</v>
       </c>
       <c r="H23" s="3">
-        <f>D23/B23</f>
+        <f t="shared" ref="H23:H32" si="6">D23/B23</f>
         <v>0.6671009771986971</v>
       </c>
       <c r="I23" s="6">
-        <f>F23*LN(G23)</f>
+        <f t="shared" ref="I23:I32" si="7">F23*LN(G23)</f>
         <v>0.28898160479624418</v>
       </c>
       <c r="J23" t="s">
@@ -1093,22 +1092,22 @@
         <v>4096</v>
       </c>
       <c r="E24" s="5">
-        <f>C24*$B$20</f>
+        <f t="shared" si="4"/>
         <v>7374100999.999999</v>
       </c>
       <c r="F24" s="3">
         <v>0.05</v>
       </c>
       <c r="G24" s="5">
-        <f>E24/C24</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H24" s="3">
-        <f>D24/B24</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I24" s="6">
-        <f>F24*LN(G24)</f>
+        <f t="shared" si="7"/>
         <v>0.14449080239812209</v>
       </c>
       <c r="J24" t="s">
@@ -1129,22 +1128,22 @@
         <v>4096</v>
       </c>
       <c r="E25" s="5">
-        <f>C25*$B$20</f>
+        <f t="shared" si="4"/>
         <v>1871139899.9999998</v>
       </c>
       <c r="F25" s="3">
         <v>0.05</v>
       </c>
       <c r="G25" s="5">
-        <f>E25/C25</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H25" s="3">
-        <f>D25/B25</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I25" s="6">
-        <f>F25*LN(G25)</f>
+        <f t="shared" si="7"/>
         <v>0.14449080239812209</v>
       </c>
       <c r="J25" t="s">
@@ -1165,22 +1164,22 @@
         <v>4096</v>
       </c>
       <c r="E26" s="5">
-        <f>C26*$B$20</f>
+        <f t="shared" si="4"/>
         <v>165328.99949999998</v>
       </c>
       <c r="F26" s="3">
         <v>0.15</v>
       </c>
       <c r="G26" s="5">
-        <f>E26/C26</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H26" s="3">
-        <f>D26/B26</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I26" s="6">
-        <f>F26*LN(G26)</f>
+        <f t="shared" si="7"/>
         <v>0.43347240719436625</v>
       </c>
       <c r="J26" t="s">
@@ -1194,7 +1193,7 @@
       <c r="B27" s="3">
         <v>6140</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27">
         <f>1/2.63468153</f>
         <v>0.37955251464491041</v>
       </c>
@@ -1202,22 +1201,22 @@
         <v>4096</v>
       </c>
       <c r="E27" s="5">
-        <f>C27*$B$20</f>
+        <f t="shared" si="4"/>
         <v>6.8281497384619376</v>
       </c>
       <c r="F27" s="3">
         <v>0.05</v>
       </c>
       <c r="G27" s="5">
-        <f>E27/C27</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H27" s="3">
-        <f>D27/B27</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I27" s="6">
-        <f>F27*LN(G27)</f>
+        <f t="shared" si="7"/>
         <v>0.14449080239812209</v>
       </c>
       <c r="J27" t="s">
@@ -1238,22 +1237,22 @@
         <v>4096</v>
       </c>
       <c r="E28" s="5">
-        <f>C28*$B$20</f>
+        <f t="shared" si="4"/>
         <v>21713.929999999997</v>
       </c>
       <c r="F28" s="3">
         <v>0.05</v>
       </c>
       <c r="G28" s="5">
-        <f>E28/C28</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H28" s="3">
-        <f>D28/B28</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I28" s="6">
-        <f>F28*LN(G28)</f>
+        <f t="shared" si="7"/>
         <v>0.14449080239812209</v>
       </c>
       <c r="J28" t="s">
@@ -1267,29 +1266,29 @@
       <c r="B29" s="3">
         <v>6140</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="7">
         <v>20000000</v>
       </c>
       <c r="D29" s="3">
         <v>4096</v>
       </c>
       <c r="E29" s="5">
-        <f>C29*$B$20</f>
+        <f t="shared" si="4"/>
         <v>359799999.99999994</v>
       </c>
       <c r="F29" s="3">
         <v>0.3</v>
       </c>
       <c r="G29" s="5">
-        <f>E29/C29</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H29" s="3">
-        <f>D29/B29</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I29" s="6">
-        <f>F29*LN(G29)</f>
+        <f t="shared" si="7"/>
         <v>0.8669448143887325</v>
       </c>
       <c r="J29" t="s">
@@ -1303,33 +1302,33 @@
       <c r="B30" s="3">
         <v>6140</v>
       </c>
-      <c r="C30" s="7">
-        <v>2394.9</v>
+      <c r="C30">
+        <v>2522.1403676464702</v>
       </c>
       <c r="D30" s="3">
         <v>4096</v>
       </c>
       <c r="E30" s="5">
-        <f>C30*$B$20</f>
-        <v>43084.250999999997</v>
+        <f t="shared" si="4"/>
+        <v>45373.305213959997</v>
       </c>
       <c r="F30" s="3">
         <v>0.1</v>
       </c>
       <c r="G30" s="5">
-        <f>E30/C30</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H30" s="3">
-        <f>D30/B30</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I30" s="6">
-        <f>F30*LN(G30)</f>
+        <f t="shared" si="7"/>
         <v>0.28898160479624418</v>
       </c>
       <c r="J30" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -1339,33 +1338,33 @@
       <c r="B31" s="3">
         <v>6140</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="7">
         <v>621330000</v>
       </c>
       <c r="D31" s="3">
         <v>4096</v>
       </c>
       <c r="E31" s="5">
-        <f>C31*$B$20</f>
+        <f t="shared" si="4"/>
         <v>11177726699.999998</v>
       </c>
       <c r="F31" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G31" s="5">
-        <f>E31/C31</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H31" s="3">
-        <f>D31/B31</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I31" s="6">
-        <f>F31*LN(G31)</f>
+        <f t="shared" si="7"/>
         <v>0.21673620359718312</v>
       </c>
       <c r="J31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -1375,33 +1374,33 @@
       <c r="B32" s="3">
         <v>6140</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <v>391002000</v>
       </c>
       <c r="D32" s="3">
         <v>4096</v>
       </c>
       <c r="E32" s="5">
-        <f>C32*$B$20</f>
+        <f t="shared" si="4"/>
         <v>7034125979.999999</v>
       </c>
       <c r="F32" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G32" s="5">
-        <f>E32/C32</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H32" s="3">
-        <f>D32/B32</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I32" s="6">
-        <f>F32*LN(G32)</f>
+        <f t="shared" si="7"/>
         <v>0.21673620359718312</v>
       </c>
       <c r="J32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update parthenon perf numbers and SSNI baseline draft, other minor fixes
</commit_message>
<xml_diff>
--- a/doc/sphinx/00_intro/SSNI-baseline-draft.xlsx
+++ b/doc/sphinx/00_intro/SSNI-baseline-draft.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gshipman/Documents/sid/ats-5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gshipman/Documents/sid/ats-5/benchmarks/doc/sphinx/00_intro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CD0C2D-F9A3-7B4F-BA7B-D5C7A832BA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828EB9E8-A688-F74A-97A3-2366969ABDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29220" yWindow="33500" windowWidth="23540" windowHeight="19420" xr2:uid="{CE21BE01-DC02-494E-9954-4C73F5D14895}"/>
+    <workbookView xWindow="640" yWindow="760" windowWidth="33920" windowHeight="21580" xr2:uid="{CE21BE01-DC02-494E-9954-4C73F5D14895}"/>
   </bookViews>
   <sheets>
     <sheet name="xROADS-Intel-SPR-HBM" sheetId="2" r:id="rId1"/>
@@ -215,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -223,13 +223,12 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,7 +546,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,7 +555,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -627,22 +626,22 @@
         <v>18000</v>
       </c>
       <c r="E7" s="5">
-        <f>C7*$B$4</f>
+        <f t="shared" ref="E7:E16" si="0">C7*$B$4</f>
         <v>3924227.9999999995</v>
       </c>
       <c r="F7" s="3">
         <v>0.1</v>
       </c>
       <c r="G7" s="5">
-        <f>E7/C7</f>
+        <f t="shared" ref="G7:G16" si="1">E7/C7</f>
         <v>4.0919999999999996</v>
       </c>
       <c r="H7" s="3">
-        <f>D7/B7</f>
+        <f t="shared" ref="H7:H16" si="2">D7/B7</f>
         <v>2.9315960912052117</v>
       </c>
       <c r="I7" s="6">
-        <f>F7*LN(G7)</f>
+        <f t="shared" ref="I7:I16" si="3">F7*LN(G7)</f>
         <v>0.14090338480893802</v>
       </c>
       <c r="J7" t="s">
@@ -663,22 +662,22 @@
         <v>18000</v>
       </c>
       <c r="E8" s="5">
-        <f>C8*$B$4</f>
+        <f t="shared" si="0"/>
         <v>1677310799.9999998</v>
       </c>
       <c r="F8" s="3">
         <v>0.05</v>
       </c>
       <c r="G8" s="5">
-        <f>E8/C8</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H8" s="3">
-        <f>D8/B8</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I8" s="6">
-        <f>F8*LN(G8)</f>
+        <f t="shared" si="3"/>
         <v>7.045169240446901E-2</v>
       </c>
       <c r="J8" t="s">
@@ -699,22 +698,22 @@
         <v>18000</v>
       </c>
       <c r="E9" s="5">
-        <f>C9*$B$4</f>
+        <f t="shared" si="0"/>
         <v>425608919.99999994</v>
       </c>
       <c r="F9" s="3">
         <v>0.05</v>
       </c>
       <c r="G9" s="5">
-        <f>E9/C9</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H9" s="3">
-        <f>D9/B9</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I9" s="6">
-        <f>F9*LN(G9)</f>
+        <f t="shared" si="3"/>
         <v>7.045169240446901E-2</v>
       </c>
       <c r="J9" t="s">
@@ -735,22 +734,22 @@
         <v>18000</v>
       </c>
       <c r="E10" s="5">
-        <f>C10*$B$4</f>
+        <f t="shared" si="0"/>
         <v>37605.684599999993</v>
       </c>
       <c r="F10" s="3">
         <v>0.15</v>
       </c>
       <c r="G10" s="5">
-        <f>E10/C10</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H10" s="3">
-        <f>D10/B10</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I10" s="6">
-        <f>F10*LN(G10)</f>
+        <f t="shared" si="3"/>
         <v>0.21135507721340699</v>
       </c>
       <c r="J10" t="s">
@@ -764,7 +763,7 @@
       <c r="B11" s="3">
         <v>6140</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11">
         <f>1/2.63468153</f>
         <v>0.37955251464491041</v>
       </c>
@@ -772,22 +771,22 @@
         <v>18000</v>
       </c>
       <c r="E11" s="5">
-        <f>C11*$B$4</f>
+        <f t="shared" si="0"/>
         <v>1.5531288899269733</v>
       </c>
       <c r="F11" s="3">
         <v>0.05</v>
       </c>
       <c r="G11" s="5">
-        <f>E11/C11</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H11" s="3">
-        <f>D11/B11</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I11" s="6">
-        <f>F11*LN(G11)</f>
+        <f t="shared" si="3"/>
         <v>7.045169240446901E-2</v>
       </c>
       <c r="J11" t="s">
@@ -808,22 +807,22 @@
         <v>18000</v>
       </c>
       <c r="E12" s="5">
-        <f>C12*$B$4</f>
+        <f t="shared" si="0"/>
         <v>4939.0439999999999</v>
       </c>
       <c r="F12" s="3">
         <v>0.05</v>
       </c>
       <c r="G12" s="5">
-        <f>E12/C12</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H12" s="3">
-        <f>D12/B12</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I12" s="6">
-        <f>F12*LN(G12)</f>
+        <f t="shared" si="3"/>
         <v>7.045169240446901E-2</v>
       </c>
       <c r="J12" t="s">
@@ -837,29 +836,29 @@
       <c r="B13" s="3">
         <v>6140</v>
       </c>
-      <c r="C13" s="8">
-        <v>20000000</v>
+      <c r="C13" s="7">
+        <v>26100000</v>
       </c>
       <c r="D13" s="3">
         <v>18000</v>
       </c>
       <c r="E13" s="5">
-        <f>C13*$B$4</f>
-        <v>81840000</v>
+        <f t="shared" si="0"/>
+        <v>106801199.99999999</v>
       </c>
       <c r="F13" s="3">
         <v>0.3</v>
       </c>
       <c r="G13" s="5">
-        <f>E13/C13</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H13" s="3">
-        <f>D13/B13</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I13" s="6">
-        <f>F13*LN(G13)</f>
+        <f t="shared" si="3"/>
         <v>0.42271015442681398</v>
       </c>
       <c r="J13" t="s">
@@ -873,29 +872,29 @@
       <c r="B14" s="3">
         <v>6140</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14">
         <v>2394.9</v>
       </c>
       <c r="D14" s="3">
         <v>18000</v>
       </c>
       <c r="E14" s="5">
-        <f>C14*$B$4</f>
+        <f t="shared" si="0"/>
         <v>9799.9308000000001</v>
       </c>
       <c r="F14" s="3">
         <v>0.1</v>
       </c>
       <c r="G14" s="5">
-        <f>E14/C14</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H14" s="3">
-        <f>D14/B14</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I14" s="6">
-        <f>F14*LN(G14)</f>
+        <f t="shared" si="3"/>
         <v>0.14090338480893802</v>
       </c>
       <c r="J14" t="s">
@@ -909,29 +908,29 @@
       <c r="B15" s="3">
         <v>6140</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>621330000</v>
       </c>
       <c r="D15" s="3">
         <v>18000</v>
       </c>
       <c r="E15" s="5">
-        <f>C15*$B$4</f>
+        <f t="shared" si="0"/>
         <v>2542482360</v>
       </c>
       <c r="F15" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G15" s="5">
-        <f>E15/C15</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H15" s="3">
-        <f>D15/B15</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I15" s="6">
-        <f>F15*LN(G15)</f>
+        <f t="shared" si="3"/>
         <v>0.10567753860670349</v>
       </c>
       <c r="J15" t="s">
@@ -945,29 +944,29 @@
       <c r="B16" s="3">
         <v>6140</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>391002000</v>
       </c>
       <c r="D16" s="3">
         <v>18000</v>
       </c>
       <c r="E16" s="5">
-        <f>C16*$B$4</f>
+        <f t="shared" si="0"/>
         <v>1599980183.9999998</v>
       </c>
       <c r="F16" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G16" s="5">
-        <f>E16/C16</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
       <c r="H16" s="3">
-        <f>D16/B16</f>
+        <f t="shared" si="2"/>
         <v>2.9315960912052117</v>
       </c>
       <c r="I16" s="6">
-        <f>F16*LN(G16)</f>
+        <f t="shared" si="3"/>
         <v>0.10567753860670349</v>
       </c>
       <c r="J16" t="s">
@@ -1057,22 +1056,22 @@
         <v>4096</v>
       </c>
       <c r="E23" s="5">
-        <f>C23*$B$20</f>
+        <f t="shared" ref="E23:E32" si="4">C23*$B$20</f>
         <v>17252410</v>
       </c>
       <c r="F23" s="3">
         <v>0.1</v>
       </c>
       <c r="G23" s="5">
-        <f>E23/C23</f>
+        <f t="shared" ref="G23:G32" si="5">E23/C23</f>
         <v>17.989999999999998</v>
       </c>
       <c r="H23" s="3">
-        <f>D23/B23</f>
+        <f t="shared" ref="H23:H32" si="6">D23/B23</f>
         <v>0.6671009771986971</v>
       </c>
       <c r="I23" s="6">
-        <f>F23*LN(G23)</f>
+        <f t="shared" ref="I23:I32" si="7">F23*LN(G23)</f>
         <v>0.28898160479624418</v>
       </c>
       <c r="J23" t="s">
@@ -1093,22 +1092,22 @@
         <v>4096</v>
       </c>
       <c r="E24" s="5">
-        <f>C24*$B$20</f>
+        <f t="shared" si="4"/>
         <v>7374100999.999999</v>
       </c>
       <c r="F24" s="3">
         <v>0.05</v>
       </c>
       <c r="G24" s="5">
-        <f>E24/C24</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H24" s="3">
-        <f>D24/B24</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I24" s="6">
-        <f>F24*LN(G24)</f>
+        <f t="shared" si="7"/>
         <v>0.14449080239812209</v>
       </c>
       <c r="J24" t="s">
@@ -1129,22 +1128,22 @@
         <v>4096</v>
       </c>
       <c r="E25" s="5">
-        <f>C25*$B$20</f>
+        <f t="shared" si="4"/>
         <v>1871139899.9999998</v>
       </c>
       <c r="F25" s="3">
         <v>0.05</v>
       </c>
       <c r="G25" s="5">
-        <f>E25/C25</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H25" s="3">
-        <f>D25/B25</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I25" s="6">
-        <f>F25*LN(G25)</f>
+        <f t="shared" si="7"/>
         <v>0.14449080239812209</v>
       </c>
       <c r="J25" t="s">
@@ -1165,22 +1164,22 @@
         <v>4096</v>
       </c>
       <c r="E26" s="5">
-        <f>C26*$B$20</f>
+        <f t="shared" si="4"/>
         <v>165328.99949999998</v>
       </c>
       <c r="F26" s="3">
         <v>0.15</v>
       </c>
       <c r="G26" s="5">
-        <f>E26/C26</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H26" s="3">
-        <f>D26/B26</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I26" s="6">
-        <f>F26*LN(G26)</f>
+        <f t="shared" si="7"/>
         <v>0.43347240719436625</v>
       </c>
       <c r="J26" t="s">
@@ -1194,7 +1193,7 @@
       <c r="B27" s="3">
         <v>6140</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27">
         <f>1/2.63468153</f>
         <v>0.37955251464491041</v>
       </c>
@@ -1202,22 +1201,22 @@
         <v>4096</v>
       </c>
       <c r="E27" s="5">
-        <f>C27*$B$20</f>
+        <f t="shared" si="4"/>
         <v>6.8281497384619376</v>
       </c>
       <c r="F27" s="3">
         <v>0.05</v>
       </c>
       <c r="G27" s="5">
-        <f>E27/C27</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H27" s="3">
-        <f>D27/B27</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I27" s="6">
-        <f>F27*LN(G27)</f>
+        <f t="shared" si="7"/>
         <v>0.14449080239812209</v>
       </c>
       <c r="J27" t="s">
@@ -1238,22 +1237,22 @@
         <v>4096</v>
       </c>
       <c r="E28" s="5">
-        <f>C28*$B$20</f>
+        <f t="shared" si="4"/>
         <v>21713.929999999997</v>
       </c>
       <c r="F28" s="3">
         <v>0.05</v>
       </c>
       <c r="G28" s="5">
-        <f>E28/C28</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H28" s="3">
-        <f>D28/B28</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I28" s="6">
-        <f>F28*LN(G28)</f>
+        <f t="shared" si="7"/>
         <v>0.14449080239812209</v>
       </c>
       <c r="J28" t="s">
@@ -1267,29 +1266,29 @@
       <c r="B29" s="3">
         <v>6140</v>
       </c>
-      <c r="C29" s="8">
-        <v>20000000</v>
+      <c r="C29" s="7">
+        <v>26100000</v>
       </c>
       <c r="D29" s="3">
         <v>4096</v>
       </c>
       <c r="E29" s="5">
-        <f>C29*$B$20</f>
-        <v>359799999.99999994</v>
+        <f t="shared" si="4"/>
+        <v>469538999.99999994</v>
       </c>
       <c r="F29" s="3">
         <v>0.3</v>
       </c>
       <c r="G29" s="5">
-        <f>E29/C29</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H29" s="3">
-        <f>D29/B29</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I29" s="6">
-        <f>F29*LN(G29)</f>
+        <f t="shared" si="7"/>
         <v>0.8669448143887325</v>
       </c>
       <c r="J29" t="s">
@@ -1303,29 +1302,29 @@
       <c r="B30" s="3">
         <v>6140</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30">
         <v>2394.9</v>
       </c>
       <c r="D30" s="3">
         <v>4096</v>
       </c>
       <c r="E30" s="5">
-        <f>C30*$B$20</f>
+        <f t="shared" si="4"/>
         <v>43084.250999999997</v>
       </c>
       <c r="F30" s="3">
         <v>0.1</v>
       </c>
       <c r="G30" s="5">
-        <f>E30/C30</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H30" s="3">
-        <f>D30/B30</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I30" s="6">
-        <f>F30*LN(G30)</f>
+        <f t="shared" si="7"/>
         <v>0.28898160479624418</v>
       </c>
       <c r="J30" t="s">
@@ -1339,29 +1338,29 @@
       <c r="B31" s="3">
         <v>6140</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="7">
         <v>621330000</v>
       </c>
       <c r="D31" s="3">
         <v>4096</v>
       </c>
       <c r="E31" s="5">
-        <f>C31*$B$20</f>
+        <f t="shared" si="4"/>
         <v>11177726699.999998</v>
       </c>
       <c r="F31" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G31" s="5">
-        <f>E31/C31</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H31" s="3">
-        <f>D31/B31</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I31" s="6">
-        <f>F31*LN(G31)</f>
+        <f t="shared" si="7"/>
         <v>0.21673620359718312</v>
       </c>
       <c r="J31" t="s">
@@ -1375,29 +1374,29 @@
       <c r="B32" s="3">
         <v>6140</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <v>391002000</v>
       </c>
       <c r="D32" s="3">
         <v>4096</v>
       </c>
       <c r="E32" s="5">
-        <f>C32*$B$20</f>
+        <f t="shared" si="4"/>
         <v>7034125979.999999</v>
       </c>
       <c r="F32" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G32" s="5">
-        <f>E32/C32</f>
+        <f t="shared" si="5"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H32" s="3">
-        <f>D32/B32</f>
+        <f t="shared" si="6"/>
         <v>0.6671009771986971</v>
       </c>
       <c r="I32" s="6">
-        <f>F32*LN(G32)</f>
+        <f t="shared" si="7"/>
         <v>0.21673620359718312</v>
       </c>
       <c r="J32" t="s">

</xml_diff>